<commit_message>
admin inventory add, delete ok
</commit_message>
<xml_diff>
--- a/designDocument/control sth.xlsx
+++ b/designDocument/control sth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuant\Desktop\Module1\Module1_workman\designDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C81A9B-5868-4AD2-BA51-0B4E92005468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211BD98F-CDC7-4E0A-93E5-47C3C10A69C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13550" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{28A4E6DB-3C1F-482C-99B0-229D92669B98}"/>
   </bookViews>
@@ -339,9 +339,6 @@
     <t>userInforList[index]</t>
   </si>
   <si>
-    <t>deleteItemFromItemList(index)</t>
-  </si>
-  <si>
     <t>itemList[index]</t>
   </si>
   <si>
@@ -379,6 +376,9 @@
   </si>
   <si>
     <t>randomUserIdGenerator()</t>
+  </si>
+  <si>
+    <t>deleteItemFromItemList(itemId)</t>
   </si>
 </sst>
 </file>
@@ -6639,10 +6639,10 @@
   <dimension ref="A1:T71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H44" sqref="H44"/>
+      <selection pane="bottomRight" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6757,10 +6757,10 @@
         <v>29</v>
       </c>
       <c r="H4" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="11"/>
@@ -7275,10 +7275,10 @@
         <v>94</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -7316,10 +7316,10 @@
         <v>95</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -7358,7 +7358,7 @@
         <v>43</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
@@ -7533,10 +7533,10 @@
         <v>29</v>
       </c>
       <c r="H27" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I27" s="5" t="s">
         <v>106</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>107</v>
       </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
@@ -7607,10 +7607,10 @@
         <v>29</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J29" s="17"/>
       <c r="K29" s="17"/>
@@ -7683,18 +7683,18 @@
         <v>31</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
@@ -7800,7 +7800,7 @@
         <v>75</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -7838,7 +7838,7 @@
         <v>77</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
@@ -7915,7 +7915,7 @@
         <v>31</v>
       </c>
       <c r="H37" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I37" s="22" t="s">
         <v>64</v>
@@ -7959,7 +7959,7 @@
         <v>31</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>92</v>
@@ -8137,10 +8137,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="H43" s="15" t="s">
         <v>111</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>